<commit_message>
Generation of overlay with 40 MHz Frequency
</commit_message>
<xml_diff>
--- a/vivado_prj/AFE_Serdes/Table.xlsx
+++ b/vivado_prj/AFE_Serdes/Table.xlsx
@@ -38,187 +38,187 @@
     <t>Slave High Address</t>
   </si>
   <si>
+    <t>Network 0</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>axi_dma_afe</t>
+  </si>
+  <si>
+    <t>/AXI_DMA_Real/axi_dma_afe/Data_S2MM (32 address bits : 4G)</t>
+  </si>
+  <si>
+    <t>/zynq_ultra_ps_e_0/SAXIGP6</t>
+  </si>
+  <si>
+    <t>S_AXI_LPD</t>
+  </si>
+  <si>
+    <t>LPD_DDR_LOW</t>
+  </si>
+  <si>
+    <t>0x0000_0000</t>
+  </si>
+  <si>
+    <t>2G</t>
+  </si>
+  <si>
+    <t>0x7FFF_FFFF</t>
+  </si>
+  <si>
+    <t>LPD_QSPI</t>
+  </si>
+  <si>
+    <t>0xC000_0000</t>
+  </si>
+  <si>
+    <t>512M</t>
+  </si>
+  <si>
+    <t>0xDFFF_FFFF</t>
+  </si>
+  <si>
+    <t>Excluded (2)</t>
+  </si>
+  <si>
+    <t>LPD_DDR_HIGH</t>
+  </si>
+  <si>
+    <t>LPD_LPS_OCM</t>
+  </si>
+  <si>
+    <t>0xFF00_0000</t>
+  </si>
+  <si>
+    <t>16M</t>
+  </si>
+  <si>
+    <t>0xFFFF_FFFF</t>
+  </si>
+  <si>
+    <t>axi_dma_afe_diff</t>
+  </si>
+  <si>
+    <t>/AXI_DMA_Real_Diff/axi_dma_afe_diff/Data_S2MM (32 address bits : 4G)</t>
+  </si>
+  <si>
+    <t>axi_dma_sine</t>
+  </si>
+  <si>
+    <t>/Axi_DMA/axi_dma_sine/Data_S2MM (32 address bits : 4G)</t>
+  </si>
+  <si>
     <t>Network 1</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>zynq_ultra_ps_e_0</t>
   </si>
   <si>
     <t>/zynq_ultra_ps_e_0/Data (40 address bits : 0x0080000000 [ 512M ])</t>
   </si>
   <si>
+    <t>/SlowControl/rpi_gpio/S_AXI</t>
+  </si>
+  <si>
+    <t>S_AXI</t>
+  </si>
+  <si>
+    <t>Reg</t>
+  </si>
+  <si>
+    <t>0x00_8009_0000</t>
+  </si>
+  <si>
+    <t>64K</t>
+  </si>
+  <si>
+    <t>0x00_8009_FFFF</t>
+  </si>
+  <si>
+    <t>0x00_0000_0000</t>
+  </si>
+  <si>
+    <t>0x00_0000_01FF</t>
+  </si>
+  <si>
+    <t>/Interrupt_Handler/axi_intc_0/S_AXI</t>
+  </si>
+  <si>
+    <t>s_axi</t>
+  </si>
+  <si>
+    <t>0x00_8000_0000</t>
+  </si>
+  <si>
+    <t>0x00_8000_FFFF</t>
+  </si>
+  <si>
+    <t>/SlowControl/pmod_2/S_AXI</t>
+  </si>
+  <si>
+    <t>0x00_8007_0000</t>
+  </si>
+  <si>
+    <t>0x00_8007_FFFF</t>
+  </si>
+  <si>
+    <t>/SlowControl/axi_quad_spi_0/AXI_LITE</t>
+  </si>
+  <si>
+    <t>AXI_LITE</t>
+  </si>
+  <si>
+    <t>0x00_8003_0000</t>
+  </si>
+  <si>
+    <t>0x00_8003_FFFF</t>
+  </si>
+  <si>
+    <t>0x00_0000_007F</t>
+  </si>
+  <si>
+    <t>/AXI_DMA_Real/axi_dma_afe/S_AXI_LITE</t>
+  </si>
+  <si>
+    <t>S_AXI_LITE</t>
+  </si>
+  <si>
+    <t>0x00_8002_0000</t>
+  </si>
+  <si>
+    <t>0x00_8002_FFFF</t>
+  </si>
+  <si>
+    <t>0x00_0000_03FF</t>
+  </si>
+  <si>
     <t>/SlowControl/uf_leds/S_AXI</t>
   </si>
   <si>
-    <t>S_AXI</t>
-  </si>
-  <si>
-    <t>Reg</t>
-  </si>
-  <si>
     <t>0x00_800A_0000</t>
   </si>
   <si>
-    <t>64K</t>
-  </si>
-  <si>
     <t>0x00_800A_FFFF</t>
   </si>
   <si>
-    <t>0x00_0000_0000</t>
-  </si>
-  <si>
-    <t>0x00_0000_01FF</t>
-  </si>
-  <si>
-    <t>/SlowControl/rpi_gpio/S_AXI</t>
-  </si>
-  <si>
-    <t>0x00_8009_0000</t>
-  </si>
-  <si>
-    <t>0x00_8009_FFFF</t>
-  </si>
-  <si>
-    <t>/SlowControl/pmod_2/S_AXI</t>
-  </si>
-  <si>
-    <t>0x00_8007_0000</t>
-  </si>
-  <si>
-    <t>0x00_8007_FFFF</t>
-  </si>
-  <si>
-    <t>/SlowControl/axi_quad_spi_0/AXI_LITE</t>
-  </si>
-  <si>
-    <t>AXI_LITE</t>
-  </si>
-  <si>
-    <t>0x00_8003_0000</t>
-  </si>
-  <si>
-    <t>0x00_8003_FFFF</t>
-  </si>
-  <si>
-    <t>0x00_0000_007F</t>
-  </si>
-  <si>
-    <t>/Interrupt_Handler/axi_intc_0/S_AXI</t>
-  </si>
-  <si>
-    <t>s_axi</t>
-  </si>
-  <si>
-    <t>0x00_8000_0000</t>
-  </si>
-  <si>
-    <t>0x00_8000_FFFF</t>
+    <t>/Axi_DMA/axi_dma_sine/S_AXI_LITE</t>
+  </si>
+  <si>
+    <t>0x00_8001_0000</t>
+  </si>
+  <si>
+    <t>0x00_8001_FFFF</t>
   </si>
   <si>
     <t>/AXI_DMA_Real_Diff/axi_dma_afe_diff/S_AXI_LITE</t>
   </si>
   <si>
-    <t>S_AXI_LITE</t>
-  </si>
-  <si>
     <t>0x00_8004_0000</t>
   </si>
   <si>
     <t>0x00_8004_FFFF</t>
-  </si>
-  <si>
-    <t>0x00_0000_03FF</t>
-  </si>
-  <si>
-    <t>/AXI_DMA_Real/axi_dma_afe/S_AXI_LITE</t>
-  </si>
-  <si>
-    <t>0x00_8002_0000</t>
-  </si>
-  <si>
-    <t>0x00_8002_FFFF</t>
-  </si>
-  <si>
-    <t>/Axi_DMA/axi_dma_sine/S_AXI_LITE</t>
-  </si>
-  <si>
-    <t>0x00_8001_0000</t>
-  </si>
-  <si>
-    <t>0x00_8001_FFFF</t>
-  </si>
-  <si>
-    <t>Network 0</t>
-  </si>
-  <si>
-    <t>axi_dma_sine</t>
-  </si>
-  <si>
-    <t>/Axi_DMA/axi_dma_sine/Data_S2MM (32 address bits : 4G)</t>
-  </si>
-  <si>
-    <t>Excluded (2)</t>
-  </si>
-  <si>
-    <t>/zynq_ultra_ps_e_0/SAXIGP6</t>
-  </si>
-  <si>
-    <t>S_AXI_LPD</t>
-  </si>
-  <si>
-    <t>LPD_LPS_OCM</t>
-  </si>
-  <si>
-    <t>0xFF00_0000</t>
-  </si>
-  <si>
-    <t>16M</t>
-  </si>
-  <si>
-    <t>0xFFFF_FFFF</t>
-  </si>
-  <si>
-    <t>LPD_DDR_HIGH</t>
-  </si>
-  <si>
-    <t>LPD_QSPI</t>
-  </si>
-  <si>
-    <t>0xC000_0000</t>
-  </si>
-  <si>
-    <t>512M</t>
-  </si>
-  <si>
-    <t>0xDFFF_FFFF</t>
-  </si>
-  <si>
-    <t>LPD_DDR_LOW</t>
-  </si>
-  <si>
-    <t>0x0000_0000</t>
-  </si>
-  <si>
-    <t>2G</t>
-  </si>
-  <si>
-    <t>0x7FFF_FFFF</t>
-  </si>
-  <si>
-    <t>axi_dma_afe_diff</t>
-  </si>
-  <si>
-    <t>/AXI_DMA_Real_Diff/axi_dma_afe_diff/Data_S2MM (32 address bits : 4G)</t>
-  </si>
-  <si>
-    <t>axi_dma_afe</t>
-  </si>
-  <si>
-    <t>/AXI_DMA_Real/axi_dma_afe/Data_S2MM (32 address bits : 4G)</t>
   </si>
 </sst>
 </file>
@@ -432,223 +432,223 @@
         <v>17</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" outlineLevel="3">
       <c r="A6" t="s" s="5">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s" s="2">
         <v>13</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="E6" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>22</v>
-      </c>
       <c r="G6" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" outlineLevel="3">
       <c r="A7" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" outlineLevel="4">
+      <c r="A8" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="D8" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" outlineLevel="4">
+      <c r="A9" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s" s="2">
+      <c r="C9" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="E7" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s" s="2">
+      <c r="D9" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="G7" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" outlineLevel="3">
-      <c r="A8" t="s" s="5">
+      <c r="E9" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="F9" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s" s="2">
+      <c r="G9" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" outlineLevel="1">
+      <c r="A10" t="s" s="3">
         <v>28</v>
       </c>
-      <c r="E8" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s" s="2">
+      <c r="B10" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" outlineLevel="2">
+      <c r="A11" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="G8" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" outlineLevel="3">
-      <c r="A9" t="s" s="5">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" outlineLevel="3">
-      <c r="A10" t="s" s="5">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="G10" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H10" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" outlineLevel="3">
-      <c r="A11" t="s" s="5">
-        <v>40</v>
-      </c>
       <c r="B11" t="s" s="2">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" outlineLevel="3">
       <c r="A12" t="s" s="5">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s" s="2">
         <v>14</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s" s="2">
         <v>16</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" outlineLevel="3">
+      <c r="A13" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="H12" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="D13" t="s" s="2">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" outlineLevel="1">
-      <c r="A14" t="s" s="3">
-        <v>47</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" outlineLevel="3">
+      <c r="A14" t="s" s="5">
+        <v>22</v>
       </c>
       <c r="B14" t="s" s="2">
         <v>9</v>
@@ -672,15 +672,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" outlineLevel="2">
-      <c r="A15" t="s" s="4">
-        <v>48</v>
+    <row r="15" outlineLevel="4">
+      <c r="A15" t="s" s="6">
+        <v>12</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s" s="2">
         <v>9</v>
@@ -698,67 +698,67 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" outlineLevel="3">
-      <c r="A16" t="s" s="5">
-        <v>49</v>
+    <row r="16" outlineLevel="4">
+      <c r="A16" t="s" s="6">
+        <v>12</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" outlineLevel="4">
-      <c r="A17" t="s" s="6">
-        <v>50</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" outlineLevel="1">
+      <c r="A17" t="s" s="3">
+        <v>30</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" outlineLevel="4">
-      <c r="A18" t="s" s="6">
-        <v>50</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" outlineLevel="2">
+      <c r="A18" t="s" s="4">
+        <v>31</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s" s="2">
         <v>9</v>
@@ -778,59 +778,59 @@
     </row>
     <row r="19" outlineLevel="3">
       <c r="A19" t="s" s="5">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" outlineLevel="3">
       <c r="A20" t="s" s="5">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" outlineLevel="1">
-      <c r="A21" t="s" s="3">
-        <v>65</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" outlineLevel="3">
+      <c r="A21" t="s" s="5">
+        <v>22</v>
       </c>
       <c r="B21" t="s" s="2">
         <v>9</v>
@@ -854,15 +854,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" outlineLevel="2">
-      <c r="A22" t="s" s="4">
-        <v>66</v>
+    <row r="22" outlineLevel="4">
+      <c r="A22" t="s" s="6">
+        <v>12</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s" s="2">
         <v>9</v>
@@ -880,41 +880,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" outlineLevel="3">
-      <c r="A23" t="s" s="5">
-        <v>49</v>
+    <row r="23" outlineLevel="4">
+      <c r="A23" t="s" s="6">
+        <v>12</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" outlineLevel="4">
-      <c r="A24" t="s" s="6">
-        <v>50</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>32</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s" s="2">
         <v>9</v>
@@ -932,264 +932,264 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" outlineLevel="4">
-      <c r="A25" t="s" s="6">
-        <v>50</v>
+    <row r="25" outlineLevel="1">
+      <c r="A25" t="s" s="3">
+        <v>33</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" outlineLevel="3">
-      <c r="A26" t="s" s="5">
-        <v>50</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" outlineLevel="2">
+      <c r="A26" t="s" s="4">
+        <v>34</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s" s="2">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>60</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" outlineLevel="3">
       <c r="A27" t="s" s="5">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s" s="2">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" outlineLevel="1">
-      <c r="A28" t="s" s="3">
-        <v>67</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" outlineLevel="3">
+      <c r="A28" t="s" s="5">
+        <v>43</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s" s="2">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" outlineLevel="2">
-      <c r="A29" t="s" s="4">
-        <v>68</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" outlineLevel="3">
+      <c r="A29" t="s" s="5">
+        <v>47</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s" s="2">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" outlineLevel="3">
       <c r="A30" t="s" s="5">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s" s="2">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" outlineLevel="4">
-      <c r="A31" t="s" s="6">
-        <v>50</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" outlineLevel="3">
+      <c r="A31" t="s" s="5">
+        <v>55</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s" s="2">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" outlineLevel="4">
-      <c r="A32" t="s" s="6">
-        <v>50</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" outlineLevel="3">
+      <c r="A32" t="s" s="5">
+        <v>60</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s" s="2">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" outlineLevel="3">
       <c r="A33" t="s" s="5">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E33" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F33" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H33" t="s" s="2">
         <v>59</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="H33" t="s" s="2">
-        <v>60</v>
       </c>
     </row>
     <row r="34" outlineLevel="3">
       <c r="A34" t="s" s="5">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s" s="2">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1197,16 +1197,16 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:H11"/>
     <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:H26"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Reduction in SPI communication speed, and petalinux files added to the project
</commit_message>
<xml_diff>
--- a/vivado_prj/AFE_Serdes/Table.xlsx
+++ b/vivado_prj/AFE_Serdes/Table.xlsx
@@ -44,72 +44,72 @@
     <t/>
   </si>
   <si>
+    <t>axi_dma_sine</t>
+  </si>
+  <si>
+    <t>/Axi_DMA/axi_dma_sine/Data_S2MM (32 address bits : 4G)</t>
+  </si>
+  <si>
+    <t>/zynq_ultra_ps_e_0/SAXIGP6</t>
+  </si>
+  <si>
+    <t>S_AXI_LPD</t>
+  </si>
+  <si>
+    <t>LPD_QSPI</t>
+  </si>
+  <si>
+    <t>0xC000_0000</t>
+  </si>
+  <si>
+    <t>512M</t>
+  </si>
+  <si>
+    <t>0xDFFF_FFFF</t>
+  </si>
+  <si>
+    <t>LPD_DDR_LOW</t>
+  </si>
+  <si>
+    <t>0x0000_0000</t>
+  </si>
+  <si>
+    <t>2G</t>
+  </si>
+  <si>
+    <t>0x7FFF_FFFF</t>
+  </si>
+  <si>
+    <t>Excluded (2)</t>
+  </si>
+  <si>
+    <t>LPD_DDR_HIGH</t>
+  </si>
+  <si>
+    <t>LPD_LPS_OCM</t>
+  </si>
+  <si>
+    <t>0xFF00_0000</t>
+  </si>
+  <si>
+    <t>16M</t>
+  </si>
+  <si>
+    <t>0xFFFF_FFFF</t>
+  </si>
+  <si>
+    <t>axi_dma_afe_diff</t>
+  </si>
+  <si>
+    <t>/AXI_DMA_Real_Diff/axi_dma_afe_diff/Data_S2MM (32 address bits : 4G)</t>
+  </si>
+  <si>
     <t>axi_dma_afe</t>
   </si>
   <si>
     <t>/AXI_DMA_Real/axi_dma_afe/Data_S2MM (32 address bits : 4G)</t>
   </si>
   <si>
-    <t>/zynq_ultra_ps_e_0/SAXIGP6</t>
-  </si>
-  <si>
-    <t>S_AXI_LPD</t>
-  </si>
-  <si>
-    <t>LPD_DDR_LOW</t>
-  </si>
-  <si>
-    <t>0x0000_0000</t>
-  </si>
-  <si>
-    <t>2G</t>
-  </si>
-  <si>
-    <t>0x7FFF_FFFF</t>
-  </si>
-  <si>
-    <t>LPD_QSPI</t>
-  </si>
-  <si>
-    <t>0xC000_0000</t>
-  </si>
-  <si>
-    <t>512M</t>
-  </si>
-  <si>
-    <t>0xDFFF_FFFF</t>
-  </si>
-  <si>
-    <t>Excluded (2)</t>
-  </si>
-  <si>
-    <t>LPD_DDR_HIGH</t>
-  </si>
-  <si>
-    <t>LPD_LPS_OCM</t>
-  </si>
-  <si>
-    <t>0xFF00_0000</t>
-  </si>
-  <si>
-    <t>16M</t>
-  </si>
-  <si>
-    <t>0xFFFF_FFFF</t>
-  </si>
-  <si>
-    <t>axi_dma_afe_diff</t>
-  </si>
-  <si>
-    <t>/AXI_DMA_Real_Diff/axi_dma_afe_diff/Data_S2MM (32 address bits : 4G)</t>
-  </si>
-  <si>
-    <t>axi_dma_sine</t>
-  </si>
-  <si>
-    <t>/Axi_DMA/axi_dma_sine/Data_S2MM (32 address bits : 4G)</t>
-  </si>
-  <si>
     <t>Network 1</t>
   </si>
   <si>
@@ -119,40 +119,79 @@
     <t>/zynq_ultra_ps_e_0/Data (40 address bits : 0x0080000000 [ 512M ])</t>
   </si>
   <si>
+    <t>/Interrupt_Handler/axi_intc_0/S_AXI</t>
+  </si>
+  <si>
+    <t>s_axi</t>
+  </si>
+  <si>
+    <t>Reg</t>
+  </si>
+  <si>
+    <t>0x00_8000_0000</t>
+  </si>
+  <si>
+    <t>64K</t>
+  </si>
+  <si>
+    <t>0x00_8000_FFFF</t>
+  </si>
+  <si>
+    <t>0x00_0000_0000</t>
+  </si>
+  <si>
+    <t>0x00_0000_01FF</t>
+  </si>
+  <si>
+    <t>/SlowControl/axi_quad_spi_0/AXI_LITE</t>
+  </si>
+  <si>
+    <t>AXI_LITE</t>
+  </si>
+  <si>
+    <t>0x00_8003_0000</t>
+  </si>
+  <si>
+    <t>0x00_8003_FFFF</t>
+  </si>
+  <si>
+    <t>0x00_0000_007F</t>
+  </si>
+  <si>
     <t>/SlowControl/rpi_gpio/S_AXI</t>
   </si>
   <si>
     <t>S_AXI</t>
   </si>
   <si>
-    <t>Reg</t>
-  </si>
-  <si>
     <t>0x00_8009_0000</t>
   </si>
   <si>
-    <t>64K</t>
-  </si>
-  <si>
     <t>0x00_8009_FFFF</t>
   </si>
   <si>
-    <t>0x00_0000_0000</t>
-  </si>
-  <si>
-    <t>0x00_0000_01FF</t>
-  </si>
-  <si>
-    <t>/Interrupt_Handler/axi_intc_0/S_AXI</t>
-  </si>
-  <si>
-    <t>s_axi</t>
-  </si>
-  <si>
-    <t>0x00_8000_0000</t>
-  </si>
-  <si>
-    <t>0x00_8000_FFFF</t>
+    <t>/Axi_DMA/axi_dma_sine/S_AXI_LITE</t>
+  </si>
+  <si>
+    <t>S_AXI_LITE</t>
+  </si>
+  <si>
+    <t>0x00_8001_0000</t>
+  </si>
+  <si>
+    <t>0x00_8001_FFFF</t>
+  </si>
+  <si>
+    <t>0x00_0000_03FF</t>
+  </si>
+  <si>
+    <t>/AXI_DMA_Real/axi_dma_afe/S_AXI_LITE</t>
+  </si>
+  <si>
+    <t>0x00_8002_0000</t>
+  </si>
+  <si>
+    <t>0x00_8002_FFFF</t>
   </si>
   <si>
     <t>/SlowControl/pmod_2/S_AXI</t>
@@ -164,36 +203,6 @@
     <t>0x00_8007_FFFF</t>
   </si>
   <si>
-    <t>/SlowControl/axi_quad_spi_0/AXI_LITE</t>
-  </si>
-  <si>
-    <t>AXI_LITE</t>
-  </si>
-  <si>
-    <t>0x00_8003_0000</t>
-  </si>
-  <si>
-    <t>0x00_8003_FFFF</t>
-  </si>
-  <si>
-    <t>0x00_0000_007F</t>
-  </si>
-  <si>
-    <t>/AXI_DMA_Real/axi_dma_afe/S_AXI_LITE</t>
-  </si>
-  <si>
-    <t>S_AXI_LITE</t>
-  </si>
-  <si>
-    <t>0x00_8002_0000</t>
-  </si>
-  <si>
-    <t>0x00_8002_FFFF</t>
-  </si>
-  <si>
-    <t>0x00_0000_03FF</t>
-  </si>
-  <si>
     <t>/SlowControl/uf_leds/S_AXI</t>
   </si>
   <si>
@@ -201,15 +210,6 @@
   </si>
   <si>
     <t>0x00_800A_FFFF</t>
-  </si>
-  <si>
-    <t>/Axi_DMA/axi_dma_sine/S_AXI_LITE</t>
-  </si>
-  <si>
-    <t>0x00_8001_0000</t>
-  </si>
-  <si>
-    <t>0x00_8001_FFFF</t>
   </si>
   <si>
     <t>/AXI_DMA_Real_Diff/axi_dma_afe_diff/S_AXI_LITE</t>
@@ -602,22 +602,22 @@
         <v>13</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" outlineLevel="3">
@@ -628,22 +628,22 @@
         <v>13</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" outlineLevel="3">
@@ -680,22 +680,22 @@
         <v>13</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" outlineLevel="4">
@@ -706,22 +706,22 @@
         <v>13</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" outlineLevel="1">
@@ -1033,27 +1033,27 @@
         <v>41</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" outlineLevel="3">
       <c r="A29" t="s" s="5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>41</v>
@@ -1064,54 +1064,54 @@
     </row>
     <row r="30" outlineLevel="3">
       <c r="A30" t="s" s="5">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>41</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" outlineLevel="3">
       <c r="A31" t="s" s="5">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E31" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>41</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" outlineLevel="3">
@@ -1119,7 +1119,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>37</v>
@@ -1145,7 +1145,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>37</v>
@@ -1163,7 +1163,7 @@
         <v>41</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" outlineLevel="3">
@@ -1171,7 +1171,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>37</v>
@@ -1189,7 +1189,7 @@
         <v>41</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>